<commit_message>
Fixed many bugs. Also implemented key word searching and adding/dropping analysis. Atom number max can be changed now. Fixed issues with CenterFit. Also we can do sine fit now.
</commit_message>
<xml_diff>
--- a/.config/becExpConfig/parameterUnit.csv.xlsx
+++ b/.config/becExpConfig/parameterUnit.csv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WOODHOUSE\Documents\Machine Code\MuscleMuseum\.config\becExpConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\MuscleMuseum\.config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85A8A25-251F-4313-924A-80D4F1DBC8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF433CE-31CE-40A9-ABA2-B1D8D0678026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>cMOT_tot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -256,23 +256,26 @@
   </si>
   <si>
     <t>ODThold</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -582,18 +585,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="4" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" customWidth="1"/>
+    <col min="3" max="4" width="12.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -601,7 +604,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -609,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -617,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -625,12 +628,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -638,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -646,7 +649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -654,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -662,7 +665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -670,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -678,7 +681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -686,7 +689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -694,7 +697,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -702,7 +705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -710,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -718,7 +721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -726,7 +729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -734,7 +737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -742,12 +745,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -755,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -763,7 +766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -771,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -779,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -787,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -795,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -803,7 +806,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -811,12 +814,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -824,7 +827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -832,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -840,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -848,7 +851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -856,7 +859,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -864,12 +867,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -877,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -885,12 +888,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -898,7 +901,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -906,7 +909,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -914,7 +917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -922,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -930,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -938,7 +941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -946,7 +949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -954,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -962,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -970,14 +973,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>55</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix description bugs. update changes in trials
</commit_message>
<xml_diff>
--- a/.config/becExpConfig/parameterUnit.csv.xlsx
+++ b/.config/becExpConfig/parameterUnit.csv.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF433CE-31CE-40A9-ABA2-B1D8D0678026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>cMOT_tot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>latticehold</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
@@ -289,7 +295,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -297,12 +303,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,20 +591,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" customWidth="1"/>
-    <col min="3" max="4" width="12.265625" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="true"/>
+    <col min="2" max="2" width="20.125" customWidth="true"/>
+    <col min="3" max="4" width="12.265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -604,7 +612,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -612,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -620,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -628,12 +636,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -641,7 +649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -649,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -657,7 +665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -665,7 +673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -673,7 +681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -681,7 +689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -689,7 +697,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -697,7 +705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -705,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -713,7 +721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -721,7 +729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -729,7 +737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -737,7 +745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -745,12 +753,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -758,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -766,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -774,7 +782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -782,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -790,7 +798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -798,7 +806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -806,7 +814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -814,12 +822,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="29" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="30" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -827,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -835,7 +843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -843,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -851,7 +859,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -859,7 +867,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -867,12 +875,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -880,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -888,12 +896,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -901,7 +909,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -909,7 +917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="42" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -917,7 +925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="43" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -925,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="44" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -933,7 +941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="45" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -941,7 +949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="46" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -949,7 +957,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="47" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -957,7 +965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="48" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -965,7 +973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="49" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -973,17 +981,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="50" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="51" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>55</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Roughly finished hardware control v1
</commit_message>
<xml_diff>
--- a/.config/becExpConfig/parameterUnit.csv.xlsx
+++ b/.config/becExpConfig/parameterUnit.csv.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\_Li\Machine Code\MuscleMuseum\.config\becExpConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\MuscleMuseum\.config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9BF97D-E7F7-48C5-AC8B-58670656A4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4FF693-C8B3-487D-A223-7D3236583C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="true"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -337,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -345,14 +345,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,18 +633,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="true"/>
-    <col min="2" max="2" width="21.5703125" customWidth="true"/>
-    <col min="3" max="4" width="12.28515625" customWidth="true"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -654,7 +652,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -662,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -670,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -678,12 +676,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -691,7 +689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -699,7 +697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -707,7 +705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -715,7 +713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -723,7 +721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -731,7 +729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -739,7 +737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -747,7 +745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -755,7 +753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -763,7 +761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -771,7 +769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -779,7 +777,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -787,7 +785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -795,12 +793,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -808,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -816,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -824,7 +822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -832,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -840,7 +838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -848,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -856,7 +854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -864,12 +862,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -877,7 +875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -885,7 +883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -893,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -901,7 +899,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -909,7 +907,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -917,12 +915,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -930,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -938,12 +936,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -951,7 +949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -959,7 +957,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -967,7 +965,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -975,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -983,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -991,7 +989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -999,7 +997,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1007,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1015,7 +1013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1023,12 +1021,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1036,7 +1034,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1044,7 +1042,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -1052,7 +1050,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1060,7 +1058,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -1068,7 +1066,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -1076,7 +1074,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -1084,12 +1082,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -1097,11 +1095,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
onsite change of hw
</commit_message>
<xml_diff>
--- a/.config/becExpConfig/parameterUnit.csv.xlsx
+++ b/.config/becExpConfig/parameterUnit.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
   <si>
     <t>cMOT_tot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -343,6 +343,18 @@
   </si>
   <si>
     <t>Rad</t>
+  </si>
+  <si>
+    <t>PTENMOTV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>MTramptime</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
@@ -669,7 +681,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView tabSelected="true" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="D61" sqref="D61"/>
@@ -1189,6 +1201,22 @@
         <v>87</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
onsite chagnes for debugging the scope
</commit_message>
<xml_diff>
--- a/.config/becExpConfig/parameterUnit.csv.xlsx
+++ b/.config/becExpConfig/parameterUnit.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\_Li\Machine Code\MuscleMuseum\.config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3545FAA8-5AAF-4EDA-AC24-E0DED40FF414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF7828A-9621-43AD-8466-D44B53D516B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1410" windowWidth="25695" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="25695" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
   <si>
     <t>cMOT_tot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>SXFTime</t>
+  </si>
+  <si>
+    <t>LatticeScope_CH1_Mean</t>
   </si>
 </sst>
 </file>
@@ -696,15 +699,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="4" width="12.28515625" customWidth="1"/>
   </cols>
@@ -1256,6 +1259,14 @@
         <v>96</v>
       </c>
     </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>